<commit_message>
Added final Self Assessment Form for IUM
</commit_message>
<xml_diff>
--- a/Self Assessment Form - IUM.xlsx
+++ b/Self Assessment Form - IUM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Desktop\TWEB_MARINO_814025_IUMTWEB12CFU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC2BEC-AA2B-467C-8EB1-5F1B618E4D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FCE3C5-7F09-4ACF-9065-2E0CC978C95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Team Name</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Giuseppe Marino</t>
-  </si>
-  <si>
-    <t>Member 4</t>
   </si>
   <si>
     <t>X</t>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>“def save_cleaned_data(dataframes, output_folder="cleanDatasets") “ che crea delle copie dei dataset, li pulisce e li inserisce in una cartella di nome cleanDatasets</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -535,17 +535,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704EA58-8849-E44F-8AE0-CB0AA8314588}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -878,20 +878,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:5" s="37" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
@@ -914,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -923,16 +923,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -962,7 +962,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="11" customFormat="1" ht="111" x14ac:dyDescent="0.45">
@@ -1041,8 +1041,8 @@
         <v>35</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="45" t="s">
-        <v>64</v>
+      <c r="E23" s="42" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
@@ -1151,7 +1151,7 @@
         <v>33</v>
       </c>
       <c r="E39" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
@@ -1231,8 +1231,8 @@
       <c r="C49" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="45" t="s">
-        <v>63</v>
+      <c r="E49" s="42" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
@@ -1303,8 +1303,8 @@
       <c r="C57" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="45" t="s">
-        <v>62</v>
+      <c r="E57" s="42" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.4">
@@ -1335,8 +1335,8 @@
       <c r="C64" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E64" s="45" t="s">
-        <v>61</v>
+      <c r="E64" s="42" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.4">
@@ -1352,8 +1352,8 @@
       <c r="C67" t="s">
         <v>21</v>
       </c>
-      <c r="E67" s="45" t="s">
-        <v>66</v>
+      <c r="E67" s="42" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.4">
@@ -1383,10 +1383,14 @@
         <v>18</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="73" x14ac:dyDescent="0.4">
       <c r="A72" s="35" t="s">

</xml_diff>

<commit_message>
(RELATED TO IUM) added new DataAnalysis using a direct integration with the Databases plus updated the other data analysis (reformatted markdown cells ),the report and the self assessment form in which I talk briefly about this direct integration.
</commit_message>
<xml_diff>
--- a/Self Assessment Form - IUM.xlsx
+++ b/Self Assessment Form - IUM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Desktop\TWEB_MARINO_814025_IUMTWEB12CFU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FCE3C5-7F09-4ACF-9065-2E0CC978C95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69147E0C-800A-45DD-90D4-84203E6B3A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Team Name</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Ho anche creato un jupyter notebook che permette l'inserimento, a piacimento dell'utente, dei dataset</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704EA58-8849-E44F-8AE0-CB0AA8314588}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1058,7 +1061,10 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.4">
@@ -1067,7 +1073,7 @@
       </c>
       <c r="C27" s="4"/>
       <c r="D27">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
@@ -1076,7 +1082,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -1085,7 +1091,7 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
@@ -1170,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.4">
       <c r="B43" s="32" t="s">
         <v>49</v>
       </c>

</xml_diff>